<commit_message>
Donorset fixed, donorset population was added
</commit_message>
<xml_diff>
--- a/public/upload/donors/2016.xlsx
+++ b/public/upload/donors/2016.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="366" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="366"/>
   </bookViews>
   <sheets>
-    <sheet name="იანვარი" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="იანვარი" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">იანვარი!$B$4:$H$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">იანვარი!$B$4:$H$57</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">იანვარი!$B$4:$H$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">იანვარი!$B$4:$H$57</definedName>
+    <definedName name="_FilterDatabase_0" localSheetId="0">იანვარი!$B$4:$H$57</definedName>
+    <definedName name="_FilterDatabase_0_0" localSheetId="0">იანვარი!$B$4:$H$57</definedName>
   </definedNames>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
@@ -733,56 +732,53 @@
     <t>top donor</t>
   </si>
   <si>
-    <t>მილერი გვენეტაძე </t>
-  </si>
-  <si>
-    <t>ტიტე ერგემლიძე </t>
-  </si>
-  <si>
-    <t>გიორგი მორგოშია </t>
-  </si>
-  <si>
-    <t>ქეთევანი შენგელია </t>
-  </si>
-  <si>
-    <t>გიორგი ქვრივიშვილი </t>
-  </si>
-  <si>
-    <t>ვახტანგ ბეგიაშვილი </t>
+    <t>მილერი გვენეტაძე</t>
+  </si>
+  <si>
+    <t>ტიტე ერგემლიძე</t>
+  </si>
+  <si>
+    <t>გიორგი მორგოშია</t>
+  </si>
+  <si>
+    <t>ქეთევანი შენგელია</t>
+  </si>
+  <si>
+    <t>გიორგი ქვრივიშვილი</t>
+  </si>
+  <si>
+    <t>ვახტანგ ბეგიაშვილი</t>
   </si>
   <si>
     <t>top party</t>
   </si>
   <si>
-    <t>გირჩი </t>
-  </si>
-  <si>
-    <t>პატრიოტთა ალიანსი </t>
-  </si>
-  <si>
-    <t>ქართული ოცნება </t>
-  </si>
-  <si>
-    <t>გაერთიანება ბედნიერი საქართველოსთვის </t>
-  </si>
-  <si>
-    <t>დევნილთა პარტია </t>
-  </si>
-  <si>
-    <t>ნაციონალური მოძრაობა </t>
+    <t>გირჩი</t>
+  </si>
+  <si>
+    <t>პატრიოტთა ალიანსი</t>
+  </si>
+  <si>
+    <t>ქართული ოცნება</t>
+  </si>
+  <si>
+    <t>გაერთიანება ბედნიერი საქართველოსთვის</t>
+  </si>
+  <si>
+    <t>დევნილთა პარტია</t>
+  </si>
+  <si>
+    <t>ნაციონალური მოძრაობა</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="M/D/YYYY"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -792,27 +788,12 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Sylfaen"/>
       <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Sylfaen"/>
@@ -820,7 +801,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Sylfaen"/>
       <family val="1"/>
@@ -841,10 +822,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -856,196 +838,426 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="15" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="true"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:H153"/>
+  <dimension ref="A1:AMK141"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E138" activeCellId="0" sqref="E138"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="3"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="14.7125506072875"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.5748987854251"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="14.7125506072875"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="70"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="13.4251012145749"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="9.1417004048583"/>
+    <col min="1" max="1" width="3" style="1"/>
+    <col min="2" max="3" width="14.7109375" style="1"/>
+    <col min="4" max="4" width="18.5703125" style="1"/>
+    <col min="5" max="6" width="14.7109375" style="1"/>
+    <col min="7" max="7" width="70" style="2"/>
+    <col min="8" max="8" width="13.42578125" style="1"/>
+    <col min="9" max="1025" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0"/>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0"/>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1"/>
+      <c r="B1"/>
+      <c r="C1"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+      <c r="H1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0"/>
-      <c r="B3" s="0"/>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
-    </row>
-    <row r="4" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+    </row>
+    <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1071,11 +1283,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7" t="n">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7">
         <v>1</v>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="B5" s="8">
         <v>42373</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -1087,7 +1299,7 @@
       <c r="E5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="10">
         <v>75</v>
       </c>
       <c r="G5" s="11" t="s">
@@ -1097,11 +1309,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7" t="n">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
         <v>2</v>
       </c>
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="8">
         <v>42373</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -1113,7 +1325,7 @@
       <c r="E6" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="10" t="n">
+      <c r="F6" s="10">
         <v>100</v>
       </c>
       <c r="G6" s="11" t="s">
@@ -1123,11 +1335,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7" t="n">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
         <v>3</v>
       </c>
-      <c r="B7" s="8" t="n">
+      <c r="B7" s="8">
         <v>42374</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -1139,7 +1351,7 @@
       <c r="E7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="10" t="n">
+      <c r="F7" s="10">
         <v>240</v>
       </c>
       <c r="G7" s="11" t="s">
@@ -1147,11 +1359,11 @@
       </c>
       <c r="H7" s="7"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7" t="n">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
         <v>4</v>
       </c>
-      <c r="B8" s="8" t="n">
+      <c r="B8" s="8">
         <v>42374</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -1163,7 +1375,7 @@
       <c r="E8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="F8" s="10" t="n">
+      <c r="F8" s="10">
         <v>500</v>
       </c>
       <c r="G8" s="11" t="s">
@@ -1173,11 +1385,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7" t="n">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
         <v>5</v>
       </c>
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="8">
         <v>42374</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -1189,7 +1401,7 @@
       <c r="E9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="10" t="n">
+      <c r="F9" s="10">
         <v>700</v>
       </c>
       <c r="G9" s="11" t="s">
@@ -1199,11 +1411,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7" t="n">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
         <v>6</v>
       </c>
-      <c r="B10" s="8" t="n">
+      <c r="B10" s="8">
         <v>42375</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -1215,7 +1427,7 @@
       <c r="E10" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="10" t="n">
+      <c r="F10" s="10">
         <v>200</v>
       </c>
       <c r="G10" s="11" t="s">
@@ -1225,11 +1437,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7" t="n">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
         <v>7</v>
       </c>
-      <c r="B11" s="8" t="n">
+      <c r="B11" s="8">
         <v>42377</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -1241,7 +1453,7 @@
       <c r="E11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="10" t="n">
+      <c r="F11" s="10">
         <v>100</v>
       </c>
       <c r="G11" s="11" t="s">
@@ -1249,11 +1461,11 @@
       </c>
       <c r="H11" s="7"/>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7" t="n">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
         <v>8</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="8">
         <v>42377</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -1265,7 +1477,7 @@
       <c r="E12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="10" t="n">
+      <c r="F12" s="10">
         <v>20</v>
       </c>
       <c r="G12" s="11" t="s">
@@ -1275,11 +1487,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7" t="n">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
         <v>9</v>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="8">
         <v>42378</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -1291,7 +1503,7 @@
       <c r="E13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="10" t="n">
+      <c r="F13" s="10">
         <v>3370</v>
       </c>
       <c r="G13" s="11" t="s">
@@ -1299,11 +1511,11 @@
       </c>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7" t="n">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
         <v>10</v>
       </c>
-      <c r="B14" s="8" t="n">
+      <c r="B14" s="8">
         <v>42380</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -1315,7 +1527,7 @@
       <c r="E14" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="F14" s="10" t="n">
+      <c r="F14" s="10">
         <v>120</v>
       </c>
       <c r="G14" s="11" t="s">
@@ -1323,11 +1535,11 @@
       </c>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="n">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
         <v>11</v>
       </c>
-      <c r="B15" s="8" t="n">
+      <c r="B15" s="8">
         <v>42380</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -1339,7 +1551,7 @@
       <c r="E15" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="F15" s="10" t="n">
+      <c r="F15" s="10">
         <v>3300</v>
       </c>
       <c r="G15" s="11" t="s">
@@ -1347,11 +1559,11 @@
       </c>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="n">
-        <v>12</v>
-      </c>
-      <c r="B16" s="8" t="n">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>12</v>
+      </c>
+      <c r="B16" s="8">
         <v>42381</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -1363,7 +1575,7 @@
       <c r="E16" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="10" t="n">
+      <c r="F16" s="10">
         <v>9</v>
       </c>
       <c r="G16" s="11" t="s">
@@ -1373,11 +1585,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="n">
-        <v>13</v>
-      </c>
-      <c r="B17" s="8" t="n">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>13</v>
+      </c>
+      <c r="B17" s="8">
         <v>42383</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -1389,7 +1601,7 @@
       <c r="E17" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="10" t="n">
+      <c r="F17" s="10">
         <v>10000</v>
       </c>
       <c r="G17" s="11" t="s">
@@ -1397,11 +1609,11 @@
       </c>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="n">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
         <v>14</v>
       </c>
-      <c r="B18" s="8" t="n">
+      <c r="B18" s="8">
         <v>42384</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -1413,7 +1625,7 @@
       <c r="E18" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F18" s="10" t="n">
+      <c r="F18" s="10">
         <v>20</v>
       </c>
       <c r="G18" s="11" t="s">
@@ -1423,11 +1635,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="n">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
         <v>15</v>
       </c>
-      <c r="B19" s="8" t="n">
+      <c r="B19" s="8">
         <v>42384</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -1439,7 +1651,7 @@
       <c r="E19" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F19" s="10" t="n">
+      <c r="F19" s="10">
         <v>100</v>
       </c>
       <c r="G19" s="11" t="s">
@@ -1449,11 +1661,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="n">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
         <v>16</v>
       </c>
-      <c r="B20" s="8" t="n">
+      <c r="B20" s="8">
         <v>42385</v>
       </c>
       <c r="C20" s="9" t="s">
@@ -1465,7 +1677,7 @@
       <c r="E20" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="10" t="n">
+      <c r="F20" s="10">
         <v>5</v>
       </c>
       <c r="G20" s="11" t="s">
@@ -1473,11 +1685,11 @@
       </c>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="n">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
         <v>17</v>
       </c>
-      <c r="B21" s="8" t="n">
+      <c r="B21" s="8">
         <v>42387</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -1489,7 +1701,7 @@
       <c r="E21" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="10" t="n">
+      <c r="F21" s="10">
         <v>4000</v>
       </c>
       <c r="G21" s="11" t="s">
@@ -1497,11 +1709,11 @@
       </c>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="n">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
         <v>18</v>
       </c>
-      <c r="B22" s="8" t="n">
+      <c r="B22" s="8">
         <v>42387</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -1513,7 +1725,7 @@
       <c r="E22" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F22" s="10" t="n">
+      <c r="F22" s="10">
         <v>80</v>
       </c>
       <c r="G22" s="11" t="s">
@@ -1521,11 +1733,11 @@
       </c>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="n">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
         <v>19</v>
       </c>
-      <c r="B23" s="8" t="n">
+      <c r="B23" s="8">
         <v>42388</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -1537,7 +1749,7 @@
       <c r="E23" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F23" s="10" t="n">
+      <c r="F23" s="10">
         <v>140</v>
       </c>
       <c r="G23" s="11" t="s">
@@ -1545,11 +1757,11 @@
       </c>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="n">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
         <v>20</v>
       </c>
-      <c r="B24" s="8" t="n">
+      <c r="B24" s="8">
         <v>42389</v>
       </c>
       <c r="C24" s="9" t="s">
@@ -1561,7 +1773,7 @@
       <c r="E24" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F24" s="10" t="n">
+      <c r="F24" s="10">
         <v>10000</v>
       </c>
       <c r="G24" s="11" t="s">
@@ -1569,11 +1781,11 @@
       </c>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="7" t="n">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
         <v>21</v>
       </c>
-      <c r="B25" s="8" t="n">
+      <c r="B25" s="8">
         <v>42391</v>
       </c>
       <c r="C25" s="9" t="s">
@@ -1585,7 +1797,7 @@
       <c r="E25" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="10" t="n">
+      <c r="F25" s="10">
         <v>350</v>
       </c>
       <c r="G25" s="11" t="s">
@@ -1593,11 +1805,11 @@
       </c>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="7" t="n">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
         <v>22</v>
       </c>
-      <c r="B26" s="8" t="n">
+      <c r="B26" s="8">
         <v>42391</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -1609,7 +1821,7 @@
       <c r="E26" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="10" t="n">
+      <c r="F26" s="10">
         <v>100</v>
       </c>
       <c r="G26" s="11" t="s">
@@ -1617,11 +1829,11 @@
       </c>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="7" t="n">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
         <v>23</v>
       </c>
-      <c r="B27" s="8" t="n">
+      <c r="B27" s="8">
         <v>42391</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -1633,7 +1845,7 @@
       <c r="E27" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="10" t="n">
+      <c r="F27" s="10">
         <v>100</v>
       </c>
       <c r="G27" s="11" t="s">
@@ -1641,11 +1853,11 @@
       </c>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="7" t="n">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
         <v>24</v>
       </c>
-      <c r="B28" s="8" t="n">
+      <c r="B28" s="8">
         <v>42391</v>
       </c>
       <c r="C28" s="9" t="s">
@@ -1657,7 +1869,7 @@
       <c r="E28" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F28" s="10" t="n">
+      <c r="F28" s="10">
         <v>100</v>
       </c>
       <c r="G28" s="11" t="s">
@@ -1665,11 +1877,11 @@
       </c>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="7" t="n">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="7">
         <v>25</v>
       </c>
-      <c r="B29" s="8" t="n">
+      <c r="B29" s="8">
         <v>42391</v>
       </c>
       <c r="C29" s="9" t="s">
@@ -1681,7 +1893,7 @@
       <c r="E29" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="10" t="n">
+      <c r="F29" s="10">
         <v>100</v>
       </c>
       <c r="G29" s="11" t="s">
@@ -1691,11 +1903,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7" t="n">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
         <v>26</v>
       </c>
-      <c r="B30" s="8" t="n">
+      <c r="B30" s="8">
         <v>42393</v>
       </c>
       <c r="C30" s="9" t="s">
@@ -1707,7 +1919,7 @@
       <c r="E30" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F30" s="10" t="n">
+      <c r="F30" s="10">
         <v>100</v>
       </c>
       <c r="G30" s="11" t="s">
@@ -1717,11 +1929,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="n">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="7">
         <v>27</v>
       </c>
-      <c r="B31" s="8" t="n">
+      <c r="B31" s="8">
         <v>42394</v>
       </c>
       <c r="C31" s="9" t="s">
@@ -1733,7 +1945,7 @@
       <c r="E31" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F31" s="10" t="n">
+      <c r="F31" s="10">
         <v>500</v>
       </c>
       <c r="G31" s="11" t="s">
@@ -1741,11 +1953,11 @@
       </c>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="n">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="7">
         <v>28</v>
       </c>
-      <c r="B32" s="8" t="n">
+      <c r="B32" s="8">
         <v>42394</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -1757,7 +1969,7 @@
       <c r="E32" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="10" t="n">
+      <c r="F32" s="10">
         <v>100</v>
       </c>
       <c r="G32" s="11" t="s">
@@ -1765,11 +1977,11 @@
       </c>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="n">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="7">
         <v>29</v>
       </c>
-      <c r="B33" s="8" t="n">
+      <c r="B33" s="8">
         <v>42394</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -1781,7 +1993,7 @@
       <c r="E33" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="F33" s="10" t="n">
+      <c r="F33" s="10">
         <v>100</v>
       </c>
       <c r="G33" s="11" t="s">
@@ -1789,11 +2001,11 @@
       </c>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="n">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="7">
         <v>30</v>
       </c>
-      <c r="B34" s="8" t="n">
+      <c r="B34" s="8">
         <v>42394</v>
       </c>
       <c r="C34" s="9" t="s">
@@ -1805,7 +2017,7 @@
       <c r="E34" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F34" s="10" t="n">
+      <c r="F34" s="10">
         <v>33</v>
       </c>
       <c r="G34" s="11" t="s">
@@ -1815,11 +2027,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="n">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="7">
         <v>31</v>
       </c>
-      <c r="B35" s="8" t="n">
+      <c r="B35" s="8">
         <v>42394</v>
       </c>
       <c r="C35" s="9" t="s">
@@ -1831,7 +2043,7 @@
       <c r="E35" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F35" s="10" t="n">
+      <c r="F35" s="10">
         <v>33</v>
       </c>
       <c r="G35" s="11" t="s">
@@ -1841,11 +2053,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="n">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="7">
         <v>32</v>
       </c>
-      <c r="B36" s="8" t="n">
+      <c r="B36" s="8">
         <v>42394</v>
       </c>
       <c r="C36" s="9" t="s">
@@ -1857,7 +2069,7 @@
       <c r="E36" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="F36" s="10" t="n">
+      <c r="F36" s="10">
         <v>200</v>
       </c>
       <c r="G36" s="11" t="s">
@@ -1867,11 +2079,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="n">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="7">
         <v>33</v>
       </c>
-      <c r="B37" s="8" t="n">
+      <c r="B37" s="8">
         <v>42394</v>
       </c>
       <c r="C37" s="9" t="s">
@@ -1883,7 +2095,7 @@
       <c r="E37" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="F37" s="10" t="n">
+      <c r="F37" s="10">
         <v>80</v>
       </c>
       <c r="G37" s="11" t="s">
@@ -1893,11 +2105,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="n">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="7">
         <v>34</v>
       </c>
-      <c r="B38" s="8" t="n">
+      <c r="B38" s="8">
         <v>42395</v>
       </c>
       <c r="C38" s="9" t="s">
@@ -1909,7 +2121,7 @@
       <c r="E38" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F38" s="10" t="n">
+      <c r="F38" s="10">
         <v>100</v>
       </c>
       <c r="G38" s="11" t="s">
@@ -1917,11 +2129,11 @@
       </c>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="n">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="7">
         <v>35</v>
       </c>
-      <c r="B39" s="8" t="n">
+      <c r="B39" s="8">
         <v>42395</v>
       </c>
       <c r="C39" s="9" t="s">
@@ -1933,7 +2145,7 @@
       <c r="E39" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F39" s="10" t="n">
+      <c r="F39" s="10">
         <v>50</v>
       </c>
       <c r="G39" s="11" t="s">
@@ -1943,11 +2155,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="n">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="7">
         <v>36</v>
       </c>
-      <c r="B40" s="8" t="n">
+      <c r="B40" s="8">
         <v>42395</v>
       </c>
       <c r="C40" s="9" t="s">
@@ -1959,7 +2171,7 @@
       <c r="E40" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="F40" s="10" t="n">
+      <c r="F40" s="10">
         <v>40</v>
       </c>
       <c r="G40" s="11" t="s">
@@ -1969,11 +2181,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="n">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="7">
         <v>37</v>
       </c>
-      <c r="B41" s="8" t="n">
+      <c r="B41" s="8">
         <v>42395</v>
       </c>
       <c r="C41" s="9" t="s">
@@ -1985,7 +2197,7 @@
       <c r="E41" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="F41" s="10" t="n">
+      <c r="F41" s="10">
         <v>60</v>
       </c>
       <c r="G41" s="11" t="s">
@@ -1995,11 +2207,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="n">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="7">
         <v>38</v>
       </c>
-      <c r="B42" s="8" t="n">
+      <c r="B42" s="8">
         <v>42395</v>
       </c>
       <c r="C42" s="9" t="s">
@@ -2011,7 +2223,7 @@
       <c r="E42" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="F42" s="10" t="n">
+      <c r="F42" s="10">
         <v>60</v>
       </c>
       <c r="G42" s="11" t="s">
@@ -2021,11 +2233,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="n">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="7">
         <v>39</v>
       </c>
-      <c r="B43" s="8" t="n">
+      <c r="B43" s="8">
         <v>42396</v>
       </c>
       <c r="C43" s="9" t="s">
@@ -2037,7 +2249,7 @@
       <c r="E43" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F43" s="10" t="n">
+      <c r="F43" s="10">
         <v>100</v>
       </c>
       <c r="G43" s="11" t="s">
@@ -2045,11 +2257,11 @@
       </c>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="n">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
         <v>40</v>
       </c>
-      <c r="B44" s="8" t="n">
+      <c r="B44" s="8">
         <v>42396</v>
       </c>
       <c r="C44" s="9" t="s">
@@ -2061,7 +2273,7 @@
       <c r="E44" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="F44" s="10" t="n">
+      <c r="F44" s="10">
         <v>45</v>
       </c>
       <c r="G44" s="11" t="s">
@@ -2071,11 +2283,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="n">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="7">
         <v>41</v>
       </c>
-      <c r="B45" s="8" t="n">
+      <c r="B45" s="8">
         <v>42396</v>
       </c>
       <c r="C45" s="9" t="s">
@@ -2087,7 +2299,7 @@
       <c r="E45" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F45" s="10" t="n">
+      <c r="F45" s="10">
         <v>40</v>
       </c>
       <c r="G45" s="11" t="s">
@@ -2097,11 +2309,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="n">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="7">
         <v>42</v>
       </c>
-      <c r="B46" s="8" t="n">
+      <c r="B46" s="8">
         <v>42397</v>
       </c>
       <c r="C46" s="9" t="s">
@@ -2113,7 +2325,7 @@
       <c r="E46" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F46" s="9" t="n">
+      <c r="F46" s="9">
         <v>243.7</v>
       </c>
       <c r="G46" s="11" t="s">
@@ -2121,11 +2333,11 @@
       </c>
       <c r="H46" s="7"/>
     </row>
-    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="n">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="7">
         <v>43</v>
       </c>
-      <c r="B47" s="8" t="n">
+      <c r="B47" s="8">
         <v>42397</v>
       </c>
       <c r="C47" s="9" t="s">
@@ -2137,7 +2349,7 @@
       <c r="E47" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="F47" s="10" t="n">
+      <c r="F47" s="10">
         <v>45</v>
       </c>
       <c r="G47" s="11" t="s">
@@ -2147,11 +2359,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="n">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="7">
         <v>44</v>
       </c>
-      <c r="B48" s="8" t="n">
+      <c r="B48" s="8">
         <v>42397</v>
       </c>
       <c r="C48" s="9" t="s">
@@ -2163,7 +2375,7 @@
       <c r="E48" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="F48" s="10" t="n">
+      <c r="F48" s="10">
         <v>45</v>
       </c>
       <c r="G48" s="11" t="s">
@@ -2173,11 +2385,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="n">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="7">
         <v>45</v>
       </c>
-      <c r="B49" s="8" t="n">
+      <c r="B49" s="8">
         <v>42397</v>
       </c>
       <c r="C49" s="9" t="s">
@@ -2189,7 +2401,7 @@
       <c r="E49" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F49" s="10" t="n">
+      <c r="F49" s="10">
         <v>30</v>
       </c>
       <c r="G49" s="11" t="s">
@@ -2199,11 +2411,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="n">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="7">
         <v>46</v>
       </c>
-      <c r="B50" s="8" t="n">
+      <c r="B50" s="8">
         <v>42398</v>
       </c>
       <c r="C50" s="9" t="s">
@@ -2215,7 +2427,7 @@
       <c r="E50" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F50" s="10" t="n">
+      <c r="F50" s="10">
         <v>2900</v>
       </c>
       <c r="G50" s="11" t="s">
@@ -2223,11 +2435,11 @@
       </c>
       <c r="H50" s="7"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="n">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="7">
         <v>47</v>
       </c>
-      <c r="B51" s="8" t="n">
+      <c r="B51" s="8">
         <v>42398</v>
       </c>
       <c r="C51" s="9" t="s">
@@ -2239,7 +2451,7 @@
       <c r="E51" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="F51" s="10" t="n">
+      <c r="F51" s="10">
         <v>3000</v>
       </c>
       <c r="G51" s="11" t="s">
@@ -2247,11 +2459,11 @@
       </c>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="n">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="7">
         <v>48</v>
       </c>
-      <c r="B52" s="8" t="n">
+      <c r="B52" s="8">
         <v>42398</v>
       </c>
       <c r="C52" s="9" t="s">
@@ -2263,7 +2475,7 @@
       <c r="E52" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F52" s="10" t="n">
+      <c r="F52" s="10">
         <v>100</v>
       </c>
       <c r="G52" s="11" t="s">
@@ -2271,11 +2483,11 @@
       </c>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="n">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="7">
         <v>49</v>
       </c>
-      <c r="B53" s="8" t="n">
+      <c r="B53" s="8">
         <v>42398</v>
       </c>
       <c r="C53" s="9" t="s">
@@ -2287,7 +2499,7 @@
       <c r="E53" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="F53" s="10" t="n">
+      <c r="F53" s="10">
         <v>20</v>
       </c>
       <c r="G53" s="11" t="s">
@@ -2297,11 +2509,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="n">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="7">
         <v>50</v>
       </c>
-      <c r="B54" s="8" t="n">
+      <c r="B54" s="8">
         <v>42398</v>
       </c>
       <c r="C54" s="9" t="s">
@@ -2313,7 +2525,7 @@
       <c r="E54" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="10" t="n">
+      <c r="F54" s="10">
         <v>75</v>
       </c>
       <c r="G54" s="11" t="s">
@@ -2323,11 +2535,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="n">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="7">
         <v>51</v>
       </c>
-      <c r="B55" s="8" t="n">
+      <c r="B55" s="8">
         <v>42398</v>
       </c>
       <c r="C55" s="9" t="s">
@@ -2339,7 +2551,7 @@
       <c r="E55" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="F55" s="10" t="n">
+      <c r="F55" s="10">
         <v>42</v>
       </c>
       <c r="G55" s="11" t="s">
@@ -2349,11 +2561,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="n">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="7">
         <v>52</v>
       </c>
-      <c r="B56" s="8" t="n">
+      <c r="B56" s="8">
         <v>42398</v>
       </c>
       <c r="C56" s="9" t="s">
@@ -2365,7 +2577,7 @@
       <c r="E56" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="F56" s="10" t="n">
+      <c r="F56" s="10">
         <v>100</v>
       </c>
       <c r="G56" s="11" t="s">
@@ -2375,11 +2587,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="n">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="7">
         <v>53</v>
       </c>
-      <c r="B57" s="8" t="n">
+      <c r="B57" s="8">
         <v>42399</v>
       </c>
       <c r="C57" s="9" t="s">
@@ -2391,7 +2603,7 @@
       <c r="E57" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F57" s="10" t="n">
+      <c r="F57" s="10">
         <v>100</v>
       </c>
       <c r="G57" s="11" t="s">
@@ -2401,11 +2613,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="n">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="7">
         <v>54</v>
       </c>
-      <c r="B58" s="12" t="n">
+      <c r="B58" s="12">
         <v>42401</v>
       </c>
       <c r="C58" s="9" t="s">
@@ -2417,7 +2629,7 @@
       <c r="E58" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="F58" s="10" t="n">
+      <c r="F58" s="10">
         <v>100</v>
       </c>
       <c r="G58" s="13" t="s">
@@ -2425,11 +2637,11 @@
       </c>
       <c r="H58" s="9"/>
     </row>
-    <row r="59" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="n">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="7">
         <v>55</v>
       </c>
-      <c r="B59" s="12" t="n">
+      <c r="B59" s="12">
         <v>42401</v>
       </c>
       <c r="C59" s="9" t="s">
@@ -2441,7 +2653,7 @@
       <c r="E59" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="F59" s="10" t="n">
+      <c r="F59" s="10">
         <v>100</v>
       </c>
       <c r="G59" s="13" t="s">
@@ -2449,11 +2661,11 @@
       </c>
       <c r="H59" s="9"/>
     </row>
-    <row r="60" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="n">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="7">
         <v>56</v>
       </c>
-      <c r="B60" s="12" t="n">
+      <c r="B60" s="12">
         <v>42401</v>
       </c>
       <c r="C60" s="9" t="s">
@@ -2465,7 +2677,7 @@
       <c r="E60" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F60" s="10" t="n">
+      <c r="F60" s="10">
         <v>60</v>
       </c>
       <c r="G60" s="13" t="s">
@@ -2475,11 +2687,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="n">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="7">
         <v>57</v>
       </c>
-      <c r="B61" s="12" t="n">
+      <c r="B61" s="12">
         <v>42401</v>
       </c>
       <c r="C61" s="9" t="s">
@@ -2491,7 +2703,7 @@
       <c r="E61" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F61" s="10" t="n">
+      <c r="F61" s="10">
         <v>75</v>
       </c>
       <c r="G61" s="13" t="s">
@@ -2501,11 +2713,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="n">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="7">
         <v>58</v>
       </c>
-      <c r="B62" s="12" t="n">
+      <c r="B62" s="12">
         <v>42401</v>
       </c>
       <c r="C62" s="9" t="s">
@@ -2517,7 +2729,7 @@
       <c r="E62" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="F62" s="9" t="n">
+      <c r="F62" s="9">
         <v>40.5</v>
       </c>
       <c r="G62" s="13" t="s">
@@ -2527,11 +2739,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="7" t="n">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="7">
         <v>59</v>
       </c>
-      <c r="B63" s="12" t="n">
+      <c r="B63" s="12">
         <v>42401</v>
       </c>
       <c r="C63" s="9" t="s">
@@ -2543,7 +2755,7 @@
       <c r="E63" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F63" s="10" t="n">
+      <c r="F63" s="10">
         <v>100</v>
       </c>
       <c r="G63" s="13" t="s">
@@ -2553,11 +2765,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="7" t="n">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="7">
         <v>60</v>
       </c>
-      <c r="B64" s="12" t="n">
+      <c r="B64" s="12">
         <v>42401</v>
       </c>
       <c r="C64" s="9" t="s">
@@ -2569,7 +2781,7 @@
       <c r="E64" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="F64" s="10" t="n">
+      <c r="F64" s="10">
         <v>54</v>
       </c>
       <c r="G64" s="13" t="s">
@@ -2579,11 +2791,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="7" t="n">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A65" s="7">
         <v>61</v>
       </c>
-      <c r="B65" s="12" t="n">
+      <c r="B65" s="12">
         <v>42402</v>
       </c>
       <c r="C65" s="9" t="s">
@@ -2595,7 +2807,7 @@
       <c r="E65" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="F65" s="10" t="n">
+      <c r="F65" s="10">
         <v>19500</v>
       </c>
       <c r="G65" s="13" t="s">
@@ -2603,11 +2815,11 @@
       </c>
       <c r="H65" s="9"/>
     </row>
-    <row r="66" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="7" t="n">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A66" s="7">
         <v>62</v>
       </c>
-      <c r="B66" s="12" t="n">
+      <c r="B66" s="12">
         <v>42402</v>
       </c>
       <c r="C66" s="9" t="s">
@@ -2619,7 +2831,7 @@
       <c r="E66" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F66" s="10" t="n">
+      <c r="F66" s="10">
         <v>120</v>
       </c>
       <c r="G66" s="13" t="s">
@@ -2627,11 +2839,11 @@
       </c>
       <c r="H66" s="9"/>
     </row>
-    <row r="67" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="7" t="n">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A67" s="7">
         <v>63</v>
       </c>
-      <c r="B67" s="12" t="n">
+      <c r="B67" s="12">
         <v>42402</v>
       </c>
       <c r="C67" s="9" t="s">
@@ -2643,7 +2855,7 @@
       <c r="E67" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="F67" s="10" t="n">
+      <c r="F67" s="10">
         <v>50</v>
       </c>
       <c r="G67" s="13" t="s">
@@ -2653,11 +2865,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="7" t="n">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A68" s="7">
         <v>64</v>
       </c>
-      <c r="B68" s="12" t="n">
+      <c r="B68" s="12">
         <v>42403</v>
       </c>
       <c r="C68" s="9" t="s">
@@ -2669,7 +2881,7 @@
       <c r="E68" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="F68" s="10" t="n">
+      <c r="F68" s="10">
         <v>500</v>
       </c>
       <c r="G68" s="13" t="s">
@@ -2677,11 +2889,11 @@
       </c>
       <c r="H68" s="9"/>
     </row>
-    <row r="69" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="7" t="n">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A69" s="7">
         <v>65</v>
       </c>
-      <c r="B69" s="12" t="n">
+      <c r="B69" s="12">
         <v>42403</v>
       </c>
       <c r="C69" s="9" t="s">
@@ -2693,7 +2905,7 @@
       <c r="E69" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="F69" s="10" t="n">
+      <c r="F69" s="10">
         <v>6300</v>
       </c>
       <c r="G69" s="13" t="s">
@@ -2701,11 +2913,11 @@
       </c>
       <c r="H69" s="9"/>
     </row>
-    <row r="70" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="7" t="n">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A70" s="7">
         <v>66</v>
       </c>
-      <c r="B70" s="12" t="n">
+      <c r="B70" s="12">
         <v>42404</v>
       </c>
       <c r="C70" s="9" t="s">
@@ -2717,7 +2929,7 @@
       <c r="E70" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="F70" s="10" t="n">
+      <c r="F70" s="10">
         <v>13200</v>
       </c>
       <c r="G70" s="13" t="s">
@@ -2725,11 +2937,11 @@
       </c>
       <c r="H70" s="9"/>
     </row>
-    <row r="71" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="7" t="n">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A71" s="7">
         <v>67</v>
       </c>
-      <c r="B71" s="12" t="n">
+      <c r="B71" s="12">
         <v>42404</v>
       </c>
       <c r="C71" s="9" t="s">
@@ -2741,7 +2953,7 @@
       <c r="E71" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="F71" s="10" t="n">
+      <c r="F71" s="10">
         <v>123</v>
       </c>
       <c r="G71" s="13" t="s">
@@ -2751,11 +2963,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="7" t="n">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A72" s="7">
         <v>68</v>
       </c>
-      <c r="B72" s="12" t="n">
+      <c r="B72" s="12">
         <v>42405</v>
       </c>
       <c r="C72" s="9" t="s">
@@ -2767,7 +2979,7 @@
       <c r="E72" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F72" s="10" t="n">
+      <c r="F72" s="10">
         <v>100</v>
       </c>
       <c r="G72" s="13" t="s">
@@ -2775,11 +2987,11 @@
       </c>
       <c r="H72" s="9"/>
     </row>
-    <row r="73" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="7" t="n">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A73" s="7">
         <v>69</v>
       </c>
-      <c r="B73" s="12" t="n">
+      <c r="B73" s="12">
         <v>42408</v>
       </c>
       <c r="C73" s="9" t="s">
@@ -2791,7 +3003,7 @@
       <c r="E73" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="F73" s="10" t="n">
+      <c r="F73" s="10">
         <v>6900</v>
       </c>
       <c r="G73" s="13" t="s">
@@ -2799,11 +3011,11 @@
       </c>
       <c r="H73" s="9"/>
     </row>
-    <row r="74" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="7" t="n">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A74" s="7">
         <v>70</v>
       </c>
-      <c r="B74" s="12" t="n">
+      <c r="B74" s="12">
         <v>42408</v>
       </c>
       <c r="C74" s="9" t="s">
@@ -2815,7 +3027,7 @@
       <c r="E74" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F74" s="10" t="n">
+      <c r="F74" s="10">
         <v>100</v>
       </c>
       <c r="G74" s="13" t="s">
@@ -2823,11 +3035,11 @@
       </c>
       <c r="H74" s="9"/>
     </row>
-    <row r="75" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="7" t="n">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A75" s="7">
         <v>71</v>
       </c>
-      <c r="B75" s="12" t="n">
+      <c r="B75" s="12">
         <v>42408</v>
       </c>
       <c r="C75" s="9" t="s">
@@ -2839,7 +3051,7 @@
       <c r="E75" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F75" s="10" t="n">
+      <c r="F75" s="10">
         <v>20</v>
       </c>
       <c r="G75" s="13" t="s">
@@ -2849,11 +3061,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="7" t="n">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A76" s="7">
         <v>72</v>
       </c>
-      <c r="B76" s="12" t="n">
+      <c r="B76" s="12">
         <v>42409</v>
       </c>
       <c r="C76" s="9" t="s">
@@ -2865,7 +3077,7 @@
       <c r="E76" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="F76" s="10" t="n">
+      <c r="F76" s="10">
         <v>2490</v>
       </c>
       <c r="G76" s="13" t="s">
@@ -2873,11 +3085,11 @@
       </c>
       <c r="H76" s="9"/>
     </row>
-    <row r="77" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="7" t="n">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A77" s="7">
         <v>73</v>
       </c>
-      <c r="B77" s="12" t="n">
+      <c r="B77" s="12">
         <v>42409</v>
       </c>
       <c r="C77" s="9" t="s">
@@ -2889,7 +3101,7 @@
       <c r="E77" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="F77" s="10" t="n">
+      <c r="F77" s="10">
         <v>60000</v>
       </c>
       <c r="G77" s="13" t="s">
@@ -2897,11 +3109,11 @@
       </c>
       <c r="H77" s="9"/>
     </row>
-    <row r="78" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="7" t="n">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A78" s="7">
         <v>74</v>
       </c>
-      <c r="B78" s="12" t="n">
+      <c r="B78" s="12">
         <v>42410</v>
       </c>
       <c r="C78" s="9" t="s">
@@ -2913,7 +3125,7 @@
       <c r="E78" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="F78" s="10" t="n">
+      <c r="F78" s="10">
         <v>9</v>
       </c>
       <c r="G78" s="13" t="s">
@@ -2923,11 +3135,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="7" t="n">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A79" s="7">
         <v>75</v>
       </c>
-      <c r="B79" s="12" t="n">
+      <c r="B79" s="12">
         <v>42412</v>
       </c>
       <c r="C79" s="9" t="s">
@@ -2939,7 +3151,7 @@
       <c r="E79" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="F79" s="10" t="n">
+      <c r="F79" s="10">
         <v>4500</v>
       </c>
       <c r="G79" s="13" t="s">
@@ -2947,11 +3159,11 @@
       </c>
       <c r="H79" s="9"/>
     </row>
-    <row r="80" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="7" t="n">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A80" s="7">
         <v>76</v>
       </c>
-      <c r="B80" s="12" t="n">
+      <c r="B80" s="12">
         <v>42415</v>
       </c>
       <c r="C80" s="9" t="s">
@@ -2963,7 +3175,7 @@
       <c r="E80" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F80" s="10" t="n">
+      <c r="F80" s="10">
         <v>20</v>
       </c>
       <c r="G80" s="11" t="s">
@@ -2973,11 +3185,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="7" t="n">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A81" s="7">
         <v>77</v>
       </c>
-      <c r="B81" s="12" t="n">
+      <c r="B81" s="12">
         <v>42415</v>
       </c>
       <c r="C81" s="9" t="s">
@@ -2989,7 +3201,7 @@
       <c r="E81" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F81" s="10" t="n">
+      <c r="F81" s="10">
         <v>100</v>
       </c>
       <c r="G81" s="13" t="s">
@@ -2999,11 +3211,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="7" t="n">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A82" s="7">
         <v>78</v>
       </c>
-      <c r="B82" s="12" t="n">
+      <c r="B82" s="12">
         <v>42417</v>
       </c>
       <c r="C82" s="9" t="s">
@@ -3015,7 +3227,7 @@
       <c r="E82" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="F82" s="10" t="n">
+      <c r="F82" s="10">
         <v>300</v>
       </c>
       <c r="G82" s="13" t="s">
@@ -3023,11 +3235,11 @@
       </c>
       <c r="H82" s="9"/>
     </row>
-    <row r="83" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="7" t="n">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A83" s="7">
         <v>79</v>
       </c>
-      <c r="B83" s="12" t="n">
+      <c r="B83" s="12">
         <v>42418</v>
       </c>
       <c r="C83" s="9" t="s">
@@ -3039,7 +3251,7 @@
       <c r="E83" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F83" s="10" t="n">
+      <c r="F83" s="10">
         <v>80</v>
       </c>
       <c r="G83" s="13" t="s">
@@ -3047,11 +3259,11 @@
       </c>
       <c r="H83" s="9"/>
     </row>
-    <row r="84" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="7" t="n">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A84" s="7">
         <v>80</v>
       </c>
-      <c r="B84" s="12" t="n">
+      <c r="B84" s="12">
         <v>42418</v>
       </c>
       <c r="C84" s="9" t="s">
@@ -3063,7 +3275,7 @@
       <c r="E84" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="F84" s="10" t="n">
+      <c r="F84" s="10">
         <v>1385</v>
       </c>
       <c r="G84" s="13" t="s">
@@ -3071,11 +3283,11 @@
       </c>
       <c r="H84" s="9"/>
     </row>
-    <row r="85" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="7" t="n">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A85" s="7">
         <v>81</v>
       </c>
-      <c r="B85" s="12" t="n">
+      <c r="B85" s="12">
         <v>42420</v>
       </c>
       <c r="C85" s="9" t="s">
@@ -3087,7 +3299,7 @@
       <c r="E85" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="F85" s="10" t="n">
+      <c r="F85" s="10">
         <v>14500</v>
       </c>
       <c r="G85" s="13" t="s">
@@ -3095,11 +3307,11 @@
       </c>
       <c r="H85" s="9"/>
     </row>
-    <row r="86" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="7" t="n">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A86" s="7">
         <v>82</v>
       </c>
-      <c r="B86" s="12" t="n">
+      <c r="B86" s="12">
         <v>42422</v>
       </c>
       <c r="C86" s="9" t="s">
@@ -3111,7 +3323,7 @@
       <c r="E86" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="F86" s="10" t="n">
+      <c r="F86" s="10">
         <v>20000</v>
       </c>
       <c r="G86" s="13" t="s">
@@ -3119,11 +3331,11 @@
       </c>
       <c r="H86" s="9"/>
     </row>
-    <row r="87" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="7" t="n">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A87" s="7">
         <v>83</v>
       </c>
-      <c r="B87" s="12" t="n">
+      <c r="B87" s="12">
         <v>42422</v>
       </c>
       <c r="C87" s="9" t="s">
@@ -3135,7 +3347,7 @@
       <c r="E87" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F87" s="10" t="n">
+      <c r="F87" s="10">
         <v>100</v>
       </c>
       <c r="G87" s="13" t="s">
@@ -3143,11 +3355,11 @@
       </c>
       <c r="H87" s="9"/>
     </row>
-    <row r="88" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="7" t="n">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A88" s="7">
         <v>84</v>
       </c>
-      <c r="B88" s="12" t="n">
+      <c r="B88" s="12">
         <v>42422</v>
       </c>
       <c r="C88" s="9" t="s">
@@ -3159,7 +3371,7 @@
       <c r="E88" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="F88" s="10" t="n">
+      <c r="F88" s="10">
         <v>84</v>
       </c>
       <c r="G88" s="13" t="s">
@@ -3169,11 +3381,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="7" t="n">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89" s="7">
         <v>85</v>
       </c>
-      <c r="B89" s="12" t="n">
+      <c r="B89" s="12">
         <v>42423</v>
       </c>
       <c r="C89" s="9" t="s">
@@ -3185,7 +3397,7 @@
       <c r="E89" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="F89" s="10" t="n">
+      <c r="F89" s="10">
         <v>1000</v>
       </c>
       <c r="G89" s="13" t="s">
@@ -3193,11 +3405,11 @@
       </c>
       <c r="H89" s="9"/>
     </row>
-    <row r="90" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="7" t="n">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90" s="7">
         <v>86</v>
       </c>
-      <c r="B90" s="12" t="n">
+      <c r="B90" s="12">
         <v>42423</v>
       </c>
       <c r="C90" s="9" t="s">
@@ -3209,7 +3421,7 @@
       <c r="E90" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="F90" s="10" t="n">
+      <c r="F90" s="10">
         <v>50</v>
       </c>
       <c r="G90" s="13" t="s">
@@ -3219,11 +3431,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="7" t="n">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A91" s="7">
         <v>87</v>
       </c>
-      <c r="B91" s="12" t="n">
+      <c r="B91" s="12">
         <v>42423</v>
       </c>
       <c r="C91" s="9" t="s">
@@ -3235,7 +3447,7 @@
       <c r="E91" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="F91" s="10" t="n">
+      <c r="F91" s="10">
         <v>30</v>
       </c>
       <c r="G91" s="13" t="s">
@@ -3245,11 +3457,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="7" t="n">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A92" s="7">
         <v>88</v>
       </c>
-      <c r="B92" s="12" t="n">
+      <c r="B92" s="12">
         <v>42424</v>
       </c>
       <c r="C92" s="9" t="s">
@@ -3261,7 +3473,7 @@
       <c r="E92" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F92" s="10" t="n">
+      <c r="F92" s="10">
         <v>100</v>
       </c>
       <c r="G92" s="13" t="s">
@@ -3269,11 +3481,11 @@
       </c>
       <c r="H92" s="9"/>
     </row>
-    <row r="93" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="7" t="n">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93" s="7">
         <v>89</v>
       </c>
-      <c r="B93" s="12" t="n">
+      <c r="B93" s="12">
         <v>42424</v>
       </c>
       <c r="C93" s="9" t="s">
@@ -3285,7 +3497,7 @@
       <c r="E93" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="F93" s="10" t="n">
+      <c r="F93" s="10">
         <v>100</v>
       </c>
       <c r="G93" s="13" t="s">
@@ -3293,11 +3505,11 @@
       </c>
       <c r="H93" s="9"/>
     </row>
-    <row r="94" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="7" t="n">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A94" s="7">
         <v>90</v>
       </c>
-      <c r="B94" s="12" t="n">
+      <c r="B94" s="12">
         <v>42424</v>
       </c>
       <c r="C94" s="9" t="s">
@@ -3309,7 +3521,7 @@
       <c r="E94" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="F94" s="10" t="n">
+      <c r="F94" s="10">
         <v>100</v>
       </c>
       <c r="G94" s="13" t="s">
@@ -3319,11 +3531,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="7" t="n">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A95" s="7">
         <v>91</v>
       </c>
-      <c r="B95" s="12" t="n">
+      <c r="B95" s="12">
         <v>42424</v>
       </c>
       <c r="C95" s="9" t="s">
@@ -3335,7 +3547,7 @@
       <c r="E95" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F95" s="10" t="n">
+      <c r="F95" s="10">
         <v>50</v>
       </c>
       <c r="G95" s="13" t="s">
@@ -3345,11 +3557,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="7" t="n">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A96" s="7">
         <v>92</v>
       </c>
-      <c r="B96" s="12" t="n">
+      <c r="B96" s="12">
         <v>42424</v>
       </c>
       <c r="C96" s="9" t="s">
@@ -3361,7 +3573,7 @@
       <c r="E96" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F96" s="10" t="n">
+      <c r="F96" s="10">
         <v>100</v>
       </c>
       <c r="G96" s="13" t="s">
@@ -3371,11 +3583,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="7" t="n">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A97" s="7">
         <v>93</v>
       </c>
-      <c r="B97" s="12" t="n">
+      <c r="B97" s="12">
         <v>42425</v>
       </c>
       <c r="C97" s="9" t="s">
@@ -3387,7 +3599,7 @@
       <c r="E97" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F97" s="10" t="n">
+      <c r="F97" s="10">
         <v>100</v>
       </c>
       <c r="G97" s="13" t="s">
@@ -3395,11 +3607,11 @@
       </c>
       <c r="H97" s="9"/>
     </row>
-    <row r="98" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="7" t="n">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A98" s="7">
         <v>94</v>
       </c>
-      <c r="B98" s="12" t="n">
+      <c r="B98" s="12">
         <v>42425</v>
       </c>
       <c r="C98" s="9" t="s">
@@ -3411,7 +3623,7 @@
       <c r="E98" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="F98" s="10" t="n">
+      <c r="F98" s="10">
         <v>550</v>
       </c>
       <c r="G98" s="13" t="s">
@@ -3419,11 +3631,11 @@
       </c>
       <c r="H98" s="9"/>
     </row>
-    <row r="99" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="7" t="n">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A99" s="7">
         <v>95</v>
       </c>
-      <c r="B99" s="12" t="n">
+      <c r="B99" s="12">
         <v>42425</v>
       </c>
       <c r="C99" s="9" t="s">
@@ -3435,7 +3647,7 @@
       <c r="E99" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="F99" s="10" t="n">
+      <c r="F99" s="10">
         <v>59958</v>
       </c>
       <c r="G99" s="13" t="s">
@@ -3443,11 +3655,11 @@
       </c>
       <c r="H99" s="9"/>
     </row>
-    <row r="100" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="7" t="n">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A100" s="7">
         <v>96</v>
       </c>
-      <c r="B100" s="12" t="n">
+      <c r="B100" s="12">
         <v>42425</v>
       </c>
       <c r="C100" s="9" t="s">
@@ -3459,7 +3671,7 @@
       <c r="E100" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="F100" s="10" t="n">
+      <c r="F100" s="10">
         <v>33</v>
       </c>
       <c r="G100" s="13" t="s">
@@ -3469,11 +3681,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="7" t="n">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A101" s="7">
         <v>97</v>
       </c>
-      <c r="B101" s="12" t="n">
+      <c r="B101" s="12">
         <v>42426</v>
       </c>
       <c r="C101" s="9" t="s">
@@ -3485,7 +3697,7 @@
       <c r="E101" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="F101" s="10" t="n">
+      <c r="F101" s="10">
         <v>100</v>
       </c>
       <c r="G101" s="13" t="s">
@@ -3493,11 +3705,11 @@
       </c>
       <c r="H101" s="9"/>
     </row>
-    <row r="102" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="7" t="n">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A102" s="7">
         <v>98</v>
       </c>
-      <c r="B102" s="12" t="n">
+      <c r="B102" s="12">
         <v>42426</v>
       </c>
       <c r="C102" s="9" t="s">
@@ -3509,7 +3721,7 @@
       <c r="E102" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F102" s="10" t="n">
+      <c r="F102" s="10">
         <v>33</v>
       </c>
       <c r="G102" s="13" t="s">
@@ -3519,11 +3731,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="7" t="n">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A103" s="7">
         <v>99</v>
       </c>
-      <c r="B103" s="12" t="n">
+      <c r="B103" s="12">
         <v>42426</v>
       </c>
       <c r="C103" s="9" t="s">
@@ -3535,7 +3747,7 @@
       <c r="E103" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="F103" s="10" t="n">
+      <c r="F103" s="10">
         <v>20</v>
       </c>
       <c r="G103" s="13" t="s">
@@ -3545,11 +3757,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="104" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="7" t="n">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A104" s="7">
         <v>100</v>
       </c>
-      <c r="B104" s="12" t="n">
+      <c r="B104" s="12">
         <v>42426</v>
       </c>
       <c r="C104" s="9" t="s">
@@ -3561,7 +3773,7 @@
       <c r="E104" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F104" s="10" t="n">
+      <c r="F104" s="10">
         <v>75</v>
       </c>
       <c r="G104" s="13" t="s">
@@ -3571,11 +3783,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="7" t="n">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A105" s="7">
         <v>101</v>
       </c>
-      <c r="B105" s="12" t="n">
+      <c r="B105" s="12">
         <v>42428</v>
       </c>
       <c r="C105" s="9" t="s">
@@ -3587,7 +3799,7 @@
       <c r="E105" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="F105" s="10" t="n">
+      <c r="F105" s="10">
         <v>100</v>
       </c>
       <c r="G105" s="13" t="s">
@@ -3597,11 +3809,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="7" t="n">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A106" s="7">
         <v>102</v>
       </c>
-      <c r="B106" s="12" t="n">
+      <c r="B106" s="12">
         <v>42429</v>
       </c>
       <c r="C106" s="9" t="s">
@@ -3613,7 +3825,7 @@
       <c r="E106" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="F106" s="10" t="n">
+      <c r="F106" s="10">
         <v>500</v>
       </c>
       <c r="G106" s="13" t="s">
@@ -3621,11 +3833,11 @@
       </c>
       <c r="H106" s="9"/>
     </row>
-    <row r="107" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="7" t="n">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A107" s="7">
         <v>103</v>
       </c>
-      <c r="B107" s="12" t="n">
+      <c r="B107" s="12">
         <v>42429</v>
       </c>
       <c r="C107" s="9" t="s">
@@ -3637,7 +3849,7 @@
       <c r="E107" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F107" s="10" t="n">
+      <c r="F107" s="10">
         <v>100</v>
       </c>
       <c r="G107" s="13" t="s">
@@ -3645,11 +3857,11 @@
       </c>
       <c r="H107" s="9"/>
     </row>
-    <row r="108" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="7" t="n">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A108" s="7">
         <v>104</v>
       </c>
-      <c r="B108" s="12" t="n">
+      <c r="B108" s="12">
         <v>42429</v>
       </c>
       <c r="C108" s="9" t="s">
@@ -3661,7 +3873,7 @@
       <c r="E108" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F108" s="10" t="n">
+      <c r="F108" s="10">
         <v>100</v>
       </c>
       <c r="G108" s="13" t="s">
@@ -3669,11 +3881,11 @@
       </c>
       <c r="H108" s="9"/>
     </row>
-    <row r="109" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="7" t="n">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A109" s="7">
         <v>105</v>
       </c>
-      <c r="B109" s="12" t="n">
+      <c r="B109" s="12">
         <v>42429</v>
       </c>
       <c r="C109" s="9" t="s">
@@ -3685,7 +3897,7 @@
       <c r="E109" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F109" s="10" t="n">
+      <c r="F109" s="10">
         <v>40</v>
       </c>
       <c r="G109" s="13" t="s">
@@ -3695,11 +3907,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="7" t="n">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A110" s="7">
         <v>106</v>
       </c>
-      <c r="B110" s="12" t="n">
+      <c r="B110" s="12">
         <v>42429</v>
       </c>
       <c r="C110" s="9" t="s">
@@ -3711,7 +3923,7 @@
       <c r="E110" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="F110" s="10" t="n">
+      <c r="F110" s="10">
         <v>45</v>
       </c>
       <c r="G110" s="13" t="s">
@@ -3721,11 +3933,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="7" t="n">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A111" s="7">
         <v>107</v>
       </c>
-      <c r="B111" s="12" t="n">
+      <c r="B111" s="12">
         <v>42429</v>
       </c>
       <c r="C111" s="9" t="s">
@@ -3737,7 +3949,7 @@
       <c r="E111" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F111" s="10" t="n">
+      <c r="F111" s="10">
         <v>60</v>
       </c>
       <c r="G111" s="13" t="s">
@@ -3747,11 +3959,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="112" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="7" t="n">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A112" s="7">
         <v>108</v>
       </c>
-      <c r="B112" s="12" t="n">
+      <c r="B112" s="12">
         <v>42429</v>
       </c>
       <c r="C112" s="9" t="s">
@@ -3763,7 +3975,7 @@
       <c r="E112" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="F112" s="10" t="n">
+      <c r="F112" s="10">
         <v>75</v>
       </c>
       <c r="G112" s="13" t="s">
@@ -3773,11 +3985,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="113" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="7" t="n">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A113" s="7">
         <v>109</v>
       </c>
-      <c r="B113" s="12" t="n">
+      <c r="B113" s="12">
         <v>42429</v>
       </c>
       <c r="C113" s="9" t="s">
@@ -3789,7 +4001,7 @@
       <c r="E113" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="F113" s="9" t="n">
+      <c r="F113" s="9">
         <v>40.5</v>
       </c>
       <c r="G113" s="13" t="s">
@@ -3799,158 +4011,220 @@
         <v>13</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D114"/>
       <c r="E114" s="14" t="s">
         <v>235</v>
       </c>
-      <c r="F114" s="15" t="n">
-        <f aca="false">SUM(F5:F113)</f>
+      <c r="F114" s="15">
+        <f>SUM(F5:F113)</f>
         <v>256640.7</v>
       </c>
-    </row>
-    <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E124" s="0"/>
-    </row>
-    <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E125" s="0"/>
-    </row>
-    <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E126" s="0"/>
-    </row>
-    <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E127" s="0"/>
-    </row>
-    <row r="128" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="G114"/>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D115"/>
+      <c r="E115"/>
+      <c r="F115"/>
+      <c r="G115"/>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D116"/>
+      <c r="E116"/>
+      <c r="F116"/>
+      <c r="G116"/>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D117"/>
+      <c r="E117"/>
+      <c r="F117"/>
+      <c r="G117"/>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D118"/>
+      <c r="E118"/>
+      <c r="F118"/>
+      <c r="G118"/>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D119"/>
+      <c r="E119"/>
+      <c r="F119"/>
+      <c r="G119"/>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D120"/>
+      <c r="E120"/>
+      <c r="F120"/>
+      <c r="G120"/>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D121"/>
+      <c r="E121"/>
+      <c r="F121"/>
+      <c r="G121"/>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D122"/>
+      <c r="E122"/>
+      <c r="F122"/>
+      <c r="G122"/>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D123"/>
+      <c r="E123"/>
+      <c r="F123"/>
+      <c r="G123"/>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D124"/>
+      <c r="E124"/>
+      <c r="F124"/>
+      <c r="G124"/>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D125"/>
+      <c r="E125"/>
+      <c r="F125"/>
+      <c r="G125"/>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D126"/>
+      <c r="E126"/>
+      <c r="F126"/>
+      <c r="G126"/>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="D127"/>
+      <c r="E127"/>
+      <c r="F127"/>
+      <c r="G127"/>
+    </row>
+    <row r="128" spans="1:8" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D128" s="1" t="s">
         <v>236</v>
       </c>
       <c r="E128" s="16"/>
-      <c r="F128" s="0"/>
-    </row>
-    <row r="129" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F128"/>
+      <c r="G128"/>
+    </row>
+    <row r="129" spans="4:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D129" s="17" t="s">
         <v>237</v>
       </c>
-      <c r="E129" s="16" t="n">
+      <c r="E129" s="16">
         <v>60000</v>
       </c>
-      <c r="F129" s="0"/>
-      <c r="G129" s="0"/>
-    </row>
-    <row r="130" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F129"/>
+      <c r="G129"/>
+    </row>
+    <row r="130" spans="4:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D130" s="17" t="s">
         <v>238</v>
       </c>
-      <c r="E130" s="16" t="n">
+      <c r="E130" s="16">
         <v>59958</v>
       </c>
-      <c r="F130" s="0"/>
-      <c r="G130" s="0"/>
-    </row>
-    <row r="131" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F130"/>
+      <c r="G130"/>
+    </row>
+    <row r="131" spans="4:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D131" s="17" t="s">
         <v>239</v>
       </c>
-      <c r="E131" s="16" t="n">
+      <c r="E131" s="16">
         <v>21000</v>
       </c>
-      <c r="F131" s="0"/>
-      <c r="G131" s="0"/>
-    </row>
-    <row r="132" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F131"/>
+      <c r="G131"/>
+    </row>
+    <row r="132" spans="4:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D132" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="E132" s="16" t="n">
+      <c r="E132" s="16">
         <v>19500</v>
       </c>
-      <c r="F132" s="0"/>
-      <c r="G132" s="0"/>
-    </row>
-    <row r="133" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F132"/>
+      <c r="G132"/>
+    </row>
+    <row r="133" spans="4:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D133" s="17" t="s">
         <v>241</v>
       </c>
-      <c r="E133" s="16" t="n">
+      <c r="E133" s="16">
         <v>14500</v>
       </c>
-      <c r="F133" s="0"/>
-      <c r="G133" s="0"/>
-    </row>
-    <row r="134" customFormat="false" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F133"/>
+      <c r="G133"/>
+    </row>
+    <row r="134" spans="4:7" ht="12.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D134" s="17" t="s">
         <v>242</v>
       </c>
-      <c r="E134" s="16" t="n">
+      <c r="E134" s="16">
         <v>13200</v>
       </c>
-      <c r="F134" s="0"/>
-      <c r="G134" s="0"/>
-    </row>
-    <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F134"/>
+      <c r="G134"/>
+    </row>
+    <row r="135" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D135" s="16" t="s">
         <v>243</v>
       </c>
-      <c r="E135" s="0"/>
-    </row>
-    <row r="136" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E135"/>
+    </row>
+    <row r="136" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D136" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="E136" s="2" t="n">
+      <c r="E136" s="2">
         <v>143058</v>
       </c>
     </row>
-    <row r="137" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="137" spans="4:7" ht="27" x14ac:dyDescent="0.3">
       <c r="D137" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="E137" s="2" t="n">
+      <c r="E137" s="2">
         <v>58603.7</v>
       </c>
     </row>
-    <row r="138" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="138" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D138" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="E138" s="2" t="n">
+      <c r="E138" s="2">
         <v>20540</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="139" spans="4:7" ht="39.75" x14ac:dyDescent="0.3">
       <c r="D139" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="E139" s="18" t="n">
+      <c r="E139" s="18">
         <v>14500</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D140" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="E140" s="18" t="n">
+      <c r="E140" s="18">
         <v>7885</v>
       </c>
     </row>
-    <row r="141" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="141" spans="4:7" ht="27" x14ac:dyDescent="0.3">
       <c r="D141" s="17" t="s">
         <v>249</v>
       </c>
-      <c r="E141" s="18" t="n">
+      <c r="E141" s="18">
         <v>5300</v>
       </c>
     </row>
-    <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="B4:H57"/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="0" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" fitToHeight="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>